<commit_message>
Cria extrator de salas para arquivos novos 😭 (que na verdade sao de semestres velhos)
</commit_message>
<xml_diff>
--- a/dados/horarios_2023_1.xlsx
+++ b/dados/horarios_2023_1.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="1026">
   <si>
-    <t xml:space="preserve">cod_ccr</t>
+    <t xml:space="preserve">cod</t>
   </si>
   <si>
     <t xml:space="preserve">nome_ccr</t>
@@ -31,13 +31,13 @@
     <t xml:space="preserve">ch_ccr</t>
   </si>
   <si>
-    <t xml:space="preserve">cursos_turma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fases_turma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expressao_horario</t>
+    <t xml:space="preserve">curso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horario</t>
   </si>
   <si>
     <t xml:space="preserve">GEX508</t>
@@ -937,7 +937,7 @@
     <t xml:space="preserve">GLA045</t>
   </si>
   <si>
-    <t xml:space="preserve">CIÊNCIAS SOCIAIS; LETRAS - PORTUGUÊS E ESPANHOL</t>
+    <t xml:space="preserve">CIÊNCIAS SOCIAIS; LETRAS</t>
   </si>
   <si>
     <t xml:space="preserve">8; 9</t>
@@ -2011,7 +2011,7 @@
     <t xml:space="preserve">ESTUDOS DA LÍNGUA PORTUGUESA V: DIVERSIDADE LINGUÍSTICA</t>
   </si>
   <si>
-    <t xml:space="preserve">LETRAS - PORTUGUÊS E ESPANHOL</t>
+    <t xml:space="preserve">LETRAS</t>
   </si>
   <si>
     <t xml:space="preserve">3T123456 (21/03/2023 - 18/04/2023), 5T123456 (23/03/2023 - 20/04/2023)</t>
@@ -2782,7 +2782,7 @@
     <t xml:space="preserve">GCH029</t>
   </si>
   <si>
-    <t xml:space="preserve">AGRONOMIA; LETRAS - PORTUGUÊS E ESPANHOL</t>
+    <t xml:space="preserve">AGRONOMIA; LETRAS</t>
   </si>
   <si>
     <t xml:space="preserve">1; 1</t>
@@ -3112,6 +3112,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3130,18 +3131,20 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
       <i val="true"/>
       <u val="single"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3185,8 +3188,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -3201,8 +3208,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Título" xfId="20"/>
-    <cellStyle name="Resultado" xfId="21"/>
+    <cellStyle name="Resultado" xfId="20"/>
+    <cellStyle name="Título" xfId="21"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -3214,16 +3221,16 @@
   </sheetPr>
   <dimension ref="A1:F472"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="119.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="60.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="60.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="295.9"/>
   </cols>
   <sheetData>

</xml_diff>